<commit_message>
Checked in by Rudy Xiong for Adding XML Dom File
</commit_message>
<xml_diff>
--- a/PSOPublicMachines.xlsx
+++ b/PSOPublicMachines.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Password</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,55 +30,99 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PC Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connection Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Domain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VDI-80-XP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cisco</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P@ssword123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rudy Xiong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Available</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Win7_16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.224.168.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cisco</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.224.168.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Win7_56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.224.168.56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cisco</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XP_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>10.224.168.18</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PC Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Connection Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Domain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VDI-80-XP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cisco</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P@ssword123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rudy Xiong</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Available</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Win7_16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.224.168.16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cisco</t>
+    <t>WebexHZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -86,7 +130,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Y</t>
+    <t>Evelyn Yao</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -94,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +153,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,26 +172,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -446,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -463,22 +492,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -489,52 +518,91 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Checked in by rudy xiong for Changing Excel to XML
</commit_message>
<xml_diff>
--- a/PSOPublicMachines.xlsx
+++ b/PSOPublicMachines.xlsx
@@ -138,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +153,13 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,18 +179,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -478,7 +493,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -549,7 +564,7 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
@@ -601,8 +616,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>